<commit_message>
Refactor state‑measure system and update experiment assets
Reworked the emotion‑regulation experiment to support fully dynamic slider geometry and tick‑based layouts across all state‑measure types. Added helper functions for unified positioning, cleaned up logging behavior, and removed unused Builder components. Converted remaining XLSX condition files to CSV, corrected mislabeled IASP image IDs, and updated the psyexp file to use the new scaling and layout logic. Improved modularity in experimentSetup and reorganized trial files for clarity.
</commit_message>
<xml_diff>
--- a/psychopy/shared/loop-templates/loopStateMeasure.xlsx
+++ b/psychopy/shared/loop-templates/loopStateMeasure.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\neuroflare-experiments\psychopy\shared\loop-templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79E74F4D-7168-4786-9462-F1A794E16654}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8384254C-D2DB-4DE4-9736-F865E0C64DAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11640" yWindow="8235" windowWidth="22845" windowHeight="10830" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -96,7 +96,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="45">
   <si>
     <t>rating_category</t>
   </si>
@@ -210,6 +210,27 @@
   </si>
   <si>
     <t>../../shared/pictures/sam-dominance.png</t>
+  </si>
+  <si>
+    <t>style</t>
+  </si>
+  <si>
+    <t>granularity</t>
+  </si>
+  <si>
+    <t>1, 2, 3, 4, 5, 6, 7, 8, 9</t>
+  </si>
+  <si>
+    <t>Rating</t>
+  </si>
+  <si>
+    <t>Radio</t>
+  </si>
+  <si>
+    <t>0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10</t>
+  </si>
+  <si>
+    <t>tick_values</t>
   </si>
 </sst>
 </file>
@@ -603,19 +624,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
+      <selection pane="bottomLeft" activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="20.7109375" style="1"/>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>32</v>
       </c>
@@ -623,19 +647,28 @@
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>12</v>
+      <c r="G1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>33</v>
       </c>
@@ -643,16 +676,25 @@
         <v>17</v>
       </c>
       <c r="C2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" t="s">
         <v>21</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>22</v>
       </c>
-      <c r="F2" t="s">
-        <v>28</v>
+      <c r="G2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
+        <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -660,16 +702,25 @@
         <v>18</v>
       </c>
       <c r="C3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" t="s">
         <v>23</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>22</v>
       </c>
-      <c r="F3" t="s">
-        <v>29</v>
+      <c r="G3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3" t="s">
+        <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>33</v>
       </c>
@@ -677,16 +728,25 @@
         <v>19</v>
       </c>
       <c r="C4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" t="s">
         <v>24</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>25</v>
       </c>
-      <c r="F4" t="s">
-        <v>30</v>
+      <c r="G4" t="s">
+        <v>43</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4" t="s">
+        <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -694,16 +754,25 @@
         <v>20</v>
       </c>
       <c r="C5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" t="s">
         <v>26</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>27</v>
       </c>
-      <c r="F5" t="s">
-        <v>31</v>
+      <c r="G5" t="s">
+        <v>43</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5" t="s">
+        <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>34</v>
       </c>
@@ -711,19 +780,28 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" t="s">
         <v>6</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>7</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>35</v>
       </c>
-      <c r="F6" t="s">
-        <v>13</v>
+      <c r="G6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6" t="s">
+        <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -731,19 +809,28 @@
         <v>4</v>
       </c>
       <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" t="s">
         <v>8</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>9</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>36</v>
       </c>
-      <c r="F7" t="s">
-        <v>14</v>
+      <c r="G7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7" t="s">
+        <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>34</v>
       </c>
@@ -751,21 +838,30 @@
         <v>5</v>
       </c>
       <c r="C8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" t="s">
         <v>10</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>11</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>37</v>
       </c>
-      <c r="F8" t="s">
-        <v>15</v>
+      <c r="G8" t="s">
+        <v>40</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid variable name" error="Variable names need to start with a letter or an underscore (_), followed by only letters, numbers and underscores." sqref="B1:D1 F1:XFD1" xr:uid="{7CD88A1A-7D71-4B66-8FF3-B42FC0AD4334}">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid variable name" error="Variable names need to start with a letter or an underscore (_), followed by only letters, numbers and underscores." sqref="B1:E1 G1:XFD1" xr:uid="{7CD88A1A-7D71-4B66-8FF3-B42FC0AD4334}">
       <formula1>AND(ISNUMBER(SUMPRODUCT(SEARCH(MID(B1,ROW(INDIRECT("1:"&amp;LEN(B1))),1),"0123456789abcdefghijklmnopqrstuvwxyzABCDEFGHIJKLMNOPQRSTUVWXYZ_"))),ISNUMBER(SEARCH(LEFT(B1,1),"abcdefghijklmnopqrstuvwxyzABCDEFGHIJKLMNOPQRSTUVWXYZ_")),NOT(ISNUMBER(SEARCH("~*",B1))))</formula1>
     </dataValidation>
   </dataValidations>
@@ -776,6 +872,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B9F5CAB0486A994CA2C3B13E059EF2AE" ma:contentTypeVersion="0" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="8645ec4a60d0c8c7009d2d6675847a91">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="636d7205651659ec4fcda0bcbde9384b">
     <xsd:element name="properties">
@@ -889,22 +1000,30 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3725960-8A89-4E70-9C40-340E0EDB6403}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3744155D-8FAB-4E67-B5E0-C7FDBFB3715D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EFF1C174-6AC6-4774-A736-3226A12360E4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -918,27 +1037,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3744155D-8FAB-4E67-B5E0-C7FDBFB3715D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3725960-8A89-4E70-9C40-340E0EDB6403}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>